<commit_message>
Project Example 2 - Corporate Rating is saved. Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 2 - Corporate Rating/Corporate Rating.xlsx
+++ b/DESIGN/rules/Example 2 - Corporate Rating/Corporate Rating.xlsx
@@ -3468,6 +3468,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3576,7 +3577,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -3584,7 +3585,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3607,7 +3608,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3682,7 +3683,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3694,13 +3695,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-0.249977111117893" rgb="FBEEC9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3712,7 +3713,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3886,9 +3887,9 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="2"/>
   </cellStyleXfs>
   <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4271,9 +4272,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4688,10 +4689,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="40.90625" customWidth="1"/>
-    <col min="6" max="6" width="56.1796875" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="13.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="40.90625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="56.1796875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -6019,8 +6020,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="57.90625" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="20.81640625" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="57.90625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
@@ -6229,11 +6230,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="24.1796875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="20.54296875" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.08984375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.35">
@@ -6448,11 +6449,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.90625" style="1"/>
-    <col min="3" max="3" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" style="1" width="8.90625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="12.6328125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="32.36328125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.54296875" collapsed="false"/>
+    <col min="6" max="16384" style="1" width="8.90625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -7046,9 +7047,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.453125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="21" width="24.08984375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -7365,11 +7366,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="15.08984375" customWidth="1"/>
-    <col min="5" max="5" width="39.36328125" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="9" max="9" width="45.6328125" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="15.08984375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="39.36328125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.6328125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="12.1796875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="45.6328125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -8010,10 +8011,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="34.81640625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="11.54296875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="21.54296875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="34.81640625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -8380,9 +8381,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="23.6328125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" style="50" width="23.6328125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="50" width="27.453125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
@@ -9128,8 +9129,8 @@
       <c r="C77" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="D77" s="53">
-        <v>2</v>
+      <c r="D77" s="53" t="n">
+        <v>1000.0</v>
       </c>
       <c r="E77" s="12"/>
       <c r="F77" s="12"/>
@@ -9199,10 +9200,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="22.08984375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.08984375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.35">
@@ -9990,9 +9991,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" style="79" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" style="79" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.1796875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="79" width="21.81640625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="79" width="17.54296875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -10234,10 +10235,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="29.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" customWidth="1"/>
-    <col min="8" max="8" width="7.453125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="29.54296875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.6328125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="6.54296875" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="7.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.35">
@@ -11140,8 +11141,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="34.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.36328125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.6328125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="22.2" thickBot="1" x14ac:dyDescent="0.5">
@@ -11301,8 +11302,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="39.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.90625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="30.08984375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
@@ -11508,11 +11509,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="12.453125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="16.1796875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="17.08984375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="10.6328125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">

</xml_diff>